<commit_message>
Team refactor and anonymise
</commit_message>
<xml_diff>
--- a/Data/2023/Lineup/Results.xlsx
+++ b/Data/2023/Lineup/Results.xlsx
@@ -832,6 +832,12 @@
       <c r="Q2" s="4">
         <v>-17</v>
       </c>
+      <c r="R2" s="4">
+        <v>15</v>
+      </c>
+      <c r="S2" s="4">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" spans="1:23">
       <c r="A3" s="3" t="s">
@@ -885,6 +891,12 @@
       <c r="Q3" s="4">
         <v>8</v>
       </c>
+      <c r="R3" s="4">
+        <v>19</v>
+      </c>
+      <c r="S3" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:23">
       <c r="A4" s="5" t="s">
@@ -938,6 +950,12 @@
       <c r="Q4" s="4">
         <v>2</v>
       </c>
+      <c r="R4" s="4">
+        <v>11</v>
+      </c>
+      <c r="S4" s="4">
+        <v>30</v>
+      </c>
     </row>
     <row r="5" spans="1:23">
       <c r="A5" s="5" t="s">
@@ -991,6 +1009,12 @@
       <c r="Q5" s="4">
         <v>0</v>
       </c>
+      <c r="R5" s="4">
+        <v>0</v>
+      </c>
+      <c r="S5" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:23">
       <c r="A6" s="5" t="s">
@@ -1044,6 +1068,12 @@
       <c r="Q6" s="4">
         <v>0</v>
       </c>
+      <c r="R6" s="4">
+        <v>0</v>
+      </c>
+      <c r="S6" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:23">
       <c r="A7" s="5" t="s">
@@ -1097,6 +1127,12 @@
       <c r="Q7" s="4">
         <v>5</v>
       </c>
+      <c r="R7" s="4">
+        <v>-16</v>
+      </c>
+      <c r="S7" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:23">
       <c r="A8" s="6" t="s">
@@ -1150,6 +1186,12 @@
       <c r="Q8" s="4">
         <v>10</v>
       </c>
+      <c r="R8" s="4">
+        <v>2</v>
+      </c>
+      <c r="S8" s="4">
+        <v>-10</v>
+      </c>
     </row>
     <row r="9" spans="1:23">
       <c r="A9" s="6" t="s">
@@ -1203,6 +1245,12 @@
       <c r="Q9" s="4">
         <v>7</v>
       </c>
+      <c r="R9" s="4">
+        <v>11</v>
+      </c>
+      <c r="S9" s="4">
+        <v>22</v>
+      </c>
     </row>
     <row r="10" spans="1:23">
       <c r="A10" s="7" t="s">
@@ -1256,6 +1304,12 @@
       <c r="Q10" s="4">
         <v>-14</v>
       </c>
+      <c r="R10" s="4">
+        <v>17</v>
+      </c>
+      <c r="S10" s="4">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" spans="1:23">
       <c r="A11" s="7" t="s">
@@ -1309,6 +1363,12 @@
       <c r="Q11" s="4">
         <v>16</v>
       </c>
+      <c r="R11" s="4">
+        <v>25</v>
+      </c>
+      <c r="S11" s="4">
+        <v>-9</v>
+      </c>
     </row>
     <row r="12" spans="1:23">
       <c r="A12" s="8" t="s">
@@ -1362,6 +1422,12 @@
       <c r="Q12" s="4">
         <v>22</v>
       </c>
+      <c r="R12" s="4">
+        <v>22</v>
+      </c>
+      <c r="S12" s="4">
+        <v>-10</v>
+      </c>
     </row>
     <row r="13" spans="1:23">
       <c r="A13" s="8" t="s">
@@ -1415,6 +1481,12 @@
       <c r="Q13" s="4">
         <v>18</v>
       </c>
+      <c r="R13" s="4">
+        <v>-14</v>
+      </c>
+      <c r="S13" s="4">
+        <v>32</v>
+      </c>
     </row>
     <row r="14" spans="1:23">
       <c r="A14" s="9" t="s">
@@ -1468,6 +1540,12 @@
       <c r="Q14" s="4">
         <v>4</v>
       </c>
+      <c r="R14" s="4">
+        <v>23</v>
+      </c>
+      <c r="S14" s="4">
+        <v>12</v>
+      </c>
     </row>
     <row r="15" spans="1:23">
       <c r="A15" s="9" t="s">
@@ -1521,6 +1599,12 @@
       <c r="Q15" s="4">
         <v>10</v>
       </c>
+      <c r="R15" s="4">
+        <v>-18</v>
+      </c>
+      <c r="S15" s="4">
+        <v>17</v>
+      </c>
     </row>
     <row r="16" spans="1:23">
       <c r="A16" s="10" t="s">
@@ -1574,6 +1658,12 @@
       <c r="Q16" s="4">
         <v>31</v>
       </c>
+      <c r="R16" s="4">
+        <v>41</v>
+      </c>
+      <c r="S16" s="4">
+        <v>46</v>
+      </c>
     </row>
     <row r="17" spans="1:23">
       <c r="A17" s="10" t="s">
@@ -1627,6 +1717,12 @@
       <c r="Q17" s="4">
         <v>35</v>
       </c>
+      <c r="R17" s="4">
+        <v>56</v>
+      </c>
+      <c r="S17" s="4">
+        <v>-20</v>
+      </c>
     </row>
     <row r="18" spans="1:23">
       <c r="A18" s="11" t="s">
@@ -1680,6 +1776,12 @@
       <c r="Q18" s="4">
         <v>20</v>
       </c>
+      <c r="R18" s="4">
+        <v>6</v>
+      </c>
+      <c r="S18" s="4">
+        <v>-4</v>
+      </c>
     </row>
     <row r="19" spans="1:23">
       <c r="A19" s="11" t="s">
@@ -1733,6 +1835,12 @@
       <c r="Q19" s="4">
         <v>14</v>
       </c>
+      <c r="R19" s="4">
+        <v>37</v>
+      </c>
+      <c r="S19" s="4">
+        <v>25</v>
+      </c>
     </row>
     <row r="20" spans="1:23">
       <c r="A20" s="12" t="s">
@@ -1786,6 +1894,12 @@
       <c r="Q20" s="4">
         <v>47</v>
       </c>
+      <c r="R20" s="4">
+        <v>62</v>
+      </c>
+      <c r="S20" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="21" spans="1:23">
       <c r="A21" s="12" t="s">
@@ -1839,6 +1953,12 @@
       <c r="Q21" s="4">
         <v>-11</v>
       </c>
+      <c r="R21" s="4">
+        <v>-3</v>
+      </c>
+      <c r="S21" s="4">
+        <v>32</v>
+      </c>
     </row>
     <row r="22" spans="1:23">
       <c r="A22" s="13" t="s">
@@ -1892,6 +2012,12 @@
       <c r="Q22" s="4">
         <v>-15</v>
       </c>
+      <c r="R22" s="4">
+        <v>23</v>
+      </c>
+      <c r="S22" s="4">
+        <v>14</v>
+      </c>
     </row>
     <row r="23" spans="1:23">
       <c r="A23" s="13" t="s">
@@ -1945,6 +2071,12 @@
       <c r="Q23" s="4">
         <v>-21</v>
       </c>
+      <c r="R23" s="4">
+        <v>-34</v>
+      </c>
+      <c r="S23" s="4">
+        <v>16</v>
+      </c>
     </row>
     <row r="25" spans="1:23">
       <c r="A25" s="1" t="s">
@@ -2069,6 +2201,12 @@
       <c r="Q26" s="4">
         <v>8.699999999999999</v>
       </c>
+      <c r="R26" s="4">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="S26" s="4">
+        <v>9.699999999999999</v>
+      </c>
     </row>
     <row r="27" spans="1:23">
       <c r="A27" s="3" t="s">
@@ -2122,6 +2260,12 @@
       <c r="Q27" s="4">
         <v>6.7</v>
       </c>
+      <c r="R27" s="4">
+        <v>7.2</v>
+      </c>
+      <c r="S27" s="4">
+        <v>7.2</v>
+      </c>
     </row>
     <row r="28" spans="1:23">
       <c r="A28" s="5" t="s">
@@ -2175,6 +2319,12 @@
       <c r="Q28" s="4">
         <v>5.4</v>
       </c>
+      <c r="R28" s="4">
+        <v>5.9</v>
+      </c>
+      <c r="S28" s="4">
+        <v>6.9</v>
+      </c>
     </row>
     <row r="29" spans="1:23">
       <c r="A29" s="5" t="s">
@@ -2228,6 +2378,12 @@
       <c r="Q29" s="4">
         <v>0</v>
       </c>
+      <c r="R29" s="4">
+        <v>0</v>
+      </c>
+      <c r="S29" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:23">
       <c r="A30" s="5" t="s">
@@ -2281,6 +2437,12 @@
       <c r="Q30" s="4">
         <v>0</v>
       </c>
+      <c r="R30" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="S30" s="4">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="31" spans="1:23">
       <c r="A31" s="5" t="s">
@@ -2334,6 +2496,12 @@
       <c r="Q31" s="4">
         <v>6</v>
       </c>
+      <c r="R31" s="4">
+        <v>0</v>
+      </c>
+      <c r="S31" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:23">
       <c r="A32" s="6" t="s">
@@ -2387,8 +2555,14 @@
       <c r="Q32" s="4">
         <v>11.5</v>
       </c>
-    </row>
-    <row r="33" spans="1:17">
+      <c r="R32" s="4">
+        <v>11.5</v>
+      </c>
+      <c r="S32" s="4">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19">
       <c r="A33" s="6" t="s">
         <v>30</v>
       </c>
@@ -2440,8 +2614,14 @@
       <c r="Q33" s="4">
         <v>11.5</v>
       </c>
-    </row>
-    <row r="34" spans="1:17">
+      <c r="R33" s="4">
+        <v>12</v>
+      </c>
+      <c r="S33" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19">
       <c r="A34" s="7" t="s">
         <v>31</v>
       </c>
@@ -2493,8 +2673,14 @@
       <c r="Q34" s="4">
         <v>10.5</v>
       </c>
-    </row>
-    <row r="35" spans="1:17">
+      <c r="R34" s="4">
+        <v>11</v>
+      </c>
+      <c r="S34" s="4">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19">
       <c r="A35" s="7" t="s">
         <v>32</v>
       </c>
@@ -2546,8 +2732,14 @@
       <c r="Q35" s="4">
         <v>14.4</v>
       </c>
-    </row>
-    <row r="36" spans="1:17">
+      <c r="R35" s="4">
+        <v>15.4</v>
+      </c>
+      <c r="S35" s="4">
+        <v>15.2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19">
       <c r="A36" s="8" t="s">
         <v>33</v>
       </c>
@@ -2599,8 +2791,14 @@
       <c r="Q36" s="4">
         <v>23</v>
       </c>
-    </row>
-    <row r="37" spans="1:17">
+      <c r="R36" s="4">
+        <v>23.3</v>
+      </c>
+      <c r="S36" s="4">
+        <v>23.1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19">
       <c r="A37" s="8" t="s">
         <v>34</v>
       </c>
@@ -2652,8 +2850,14 @@
       <c r="Q37" s="4">
         <v>19.9</v>
       </c>
-    </row>
-    <row r="38" spans="1:17">
+      <c r="R37" s="4">
+        <v>19.4</v>
+      </c>
+      <c r="S37" s="4">
+        <v>19.7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19">
       <c r="A38" s="9" t="s">
         <v>35</v>
       </c>
@@ -2705,8 +2909,14 @@
       <c r="Q38" s="4">
         <v>8.300000000000001</v>
       </c>
-    </row>
-    <row r="39" spans="1:17">
+      <c r="R38" s="4">
+        <v>9.300000000000001</v>
+      </c>
+      <c r="S38" s="4">
+        <v>9.800000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19">
       <c r="A39" s="9" t="s">
         <v>36</v>
       </c>
@@ -2758,8 +2968,14 @@
       <c r="Q39" s="4">
         <v>5.3</v>
       </c>
-    </row>
-    <row r="40" spans="1:17">
+      <c r="R39" s="4">
+        <v>5.2</v>
+      </c>
+      <c r="S39" s="4">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19">
       <c r="A40" s="10" t="s">
         <v>37</v>
       </c>
@@ -2811,8 +3027,14 @@
       <c r="Q40" s="4">
         <v>16.7</v>
       </c>
-    </row>
-    <row r="41" spans="1:17">
+      <c r="R40" s="4">
+        <v>17</v>
+      </c>
+      <c r="S40" s="4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19">
       <c r="A41" s="10" t="s">
         <v>38</v>
       </c>
@@ -2864,8 +3086,14 @@
       <c r="Q41" s="4">
         <v>12.5</v>
       </c>
-    </row>
-    <row r="42" spans="1:17">
+      <c r="R41" s="4">
+        <v>14</v>
+      </c>
+      <c r="S41" s="4">
+        <v>13.9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19">
       <c r="A42" s="11" t="s">
         <v>39</v>
       </c>
@@ -2917,8 +3145,14 @@
       <c r="Q42" s="4">
         <v>25.6</v>
       </c>
-    </row>
-    <row r="43" spans="1:17">
+      <c r="R42" s="4">
+        <v>25.3</v>
+      </c>
+      <c r="S42" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19">
       <c r="A43" s="11" t="s">
         <v>40</v>
       </c>
@@ -2970,8 +3204,14 @@
       <c r="Q43" s="4">
         <v>19.6</v>
       </c>
-    </row>
-    <row r="44" spans="1:17">
+      <c r="R43" s="4">
+        <v>19.9</v>
+      </c>
+      <c r="S43" s="4">
+        <v>20.2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19">
       <c r="A44" s="12" t="s">
         <v>41</v>
       </c>
@@ -3023,8 +3263,14 @@
       <c r="Q44" s="4">
         <v>29.1</v>
       </c>
-    </row>
-    <row r="45" spans="1:17">
+      <c r="R44" s="4">
+        <v>29.3</v>
+      </c>
+      <c r="S44" s="4">
+        <v>29.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19">
       <c r="A45" s="12" t="s">
         <v>42</v>
       </c>
@@ -3076,8 +3322,14 @@
       <c r="Q45" s="4">
         <v>20.3</v>
       </c>
-    </row>
-    <row r="46" spans="1:17">
+      <c r="R45" s="4">
+        <v>20.1</v>
+      </c>
+      <c r="S45" s="4">
+        <v>20.4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19">
       <c r="A46" s="13" t="s">
         <v>43</v>
       </c>
@@ -3129,8 +3381,14 @@
       <c r="Q46" s="4">
         <v>9.300000000000001</v>
       </c>
-    </row>
-    <row r="47" spans="1:17">
+      <c r="R46" s="4">
+        <v>10.3</v>
+      </c>
+      <c r="S46" s="4">
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19">
       <c r="A47" s="13" t="s">
         <v>44</v>
       </c>
@@ -3181,6 +3439,12 @@
       </c>
       <c r="Q47" s="4">
         <v>4.9</v>
+      </c>
+      <c r="R47" s="4">
+        <v>4.8</v>
+      </c>
+      <c r="S47" s="4">
+        <v>5.3</v>
       </c>
     </row>
     <row r="49" spans="1:23">
@@ -3306,6 +3570,12 @@
       <c r="Q50" s="4">
         <v>36</v>
       </c>
+      <c r="R50" s="4">
+        <v>51</v>
+      </c>
+      <c r="S50" s="4">
+        <v>61</v>
+      </c>
     </row>
     <row r="51" spans="1:23">
       <c r="A51" s="3" t="s">
@@ -3359,6 +3629,12 @@
       <c r="Q51" s="4">
         <v>101</v>
       </c>
+      <c r="R51" s="4">
+        <v>120</v>
+      </c>
+      <c r="S51" s="4">
+        <v>122</v>
+      </c>
     </row>
     <row r="52" spans="1:23">
       <c r="A52" s="5" t="s">
@@ -3412,6 +3688,12 @@
       <c r="Q52" s="4">
         <v>42</v>
       </c>
+      <c r="R52" s="4">
+        <v>53</v>
+      </c>
+      <c r="S52" s="4">
+        <v>83</v>
+      </c>
     </row>
     <row r="53" spans="1:23">
       <c r="A53" s="5" t="s">
@@ -3465,6 +3747,12 @@
       <c r="Q53" s="4">
         <v>20</v>
       </c>
+      <c r="R53" s="4">
+        <v>20</v>
+      </c>
+      <c r="S53" s="4">
+        <v>20</v>
+      </c>
     </row>
     <row r="54" spans="1:23">
       <c r="A54" s="6" t="s">
@@ -3518,6 +3806,12 @@
       <c r="Q54" s="4">
         <v>59</v>
       </c>
+      <c r="R54" s="4">
+        <v>61</v>
+      </c>
+      <c r="S54" s="4">
+        <v>51</v>
+      </c>
     </row>
     <row r="55" spans="1:23">
       <c r="A55" s="6" t="s">
@@ -3571,6 +3865,12 @@
       <c r="Q55" s="4">
         <v>158</v>
       </c>
+      <c r="R55" s="4">
+        <v>169</v>
+      </c>
+      <c r="S55" s="4">
+        <v>191</v>
+      </c>
     </row>
     <row r="56" spans="1:23">
       <c r="A56" s="7" t="s">
@@ -3624,6 +3924,12 @@
       <c r="Q56" s="4">
         <v>118</v>
       </c>
+      <c r="R56" s="4">
+        <v>135</v>
+      </c>
+      <c r="S56" s="4">
+        <v>145</v>
+      </c>
     </row>
     <row r="57" spans="1:23">
       <c r="A57" s="7" t="s">
@@ -3677,6 +3983,12 @@
       <c r="Q57" s="4">
         <v>336</v>
       </c>
+      <c r="R57" s="4">
+        <v>361</v>
+      </c>
+      <c r="S57" s="4">
+        <v>352</v>
+      </c>
     </row>
     <row r="58" spans="1:23">
       <c r="A58" s="8" t="s">
@@ -3730,6 +4042,12 @@
       <c r="Q58" s="4">
         <v>232</v>
       </c>
+      <c r="R58" s="4">
+        <v>254</v>
+      </c>
+      <c r="S58" s="4">
+        <v>244</v>
+      </c>
     </row>
     <row r="59" spans="1:23">
       <c r="A59" s="8" t="s">
@@ -3783,6 +4101,12 @@
       <c r="Q59" s="4">
         <v>298</v>
       </c>
+      <c r="R59" s="4">
+        <v>284</v>
+      </c>
+      <c r="S59" s="4">
+        <v>316</v>
+      </c>
     </row>
     <row r="60" spans="1:23">
       <c r="A60" s="9" t="s">
@@ -3836,6 +4160,12 @@
       <c r="Q60" s="4">
         <v>86</v>
       </c>
+      <c r="R60" s="4">
+        <v>109</v>
+      </c>
+      <c r="S60" s="4">
+        <v>121</v>
+      </c>
     </row>
     <row r="61" spans="1:23">
       <c r="A61" s="9" t="s">
@@ -3889,6 +4219,12 @@
       <c r="Q61" s="4">
         <v>54</v>
       </c>
+      <c r="R61" s="4">
+        <v>36</v>
+      </c>
+      <c r="S61" s="4">
+        <v>53</v>
+      </c>
     </row>
     <row r="62" spans="1:23">
       <c r="A62" s="10" t="s">
@@ -3942,6 +4278,12 @@
       <c r="Q62" s="4">
         <v>238</v>
       </c>
+      <c r="R62" s="4">
+        <v>279</v>
+      </c>
+      <c r="S62" s="4">
+        <v>325</v>
+      </c>
     </row>
     <row r="63" spans="1:23">
       <c r="A63" s="10" t="s">
@@ -3995,6 +4337,12 @@
       <c r="Q63" s="4">
         <v>168</v>
       </c>
+      <c r="R63" s="4">
+        <v>224</v>
+      </c>
+      <c r="S63" s="4">
+        <v>204</v>
+      </c>
     </row>
     <row r="64" spans="1:23">
       <c r="A64" s="11" t="s">
@@ -4048,6 +4396,12 @@
       <c r="Q64" s="4">
         <v>410</v>
       </c>
+      <c r="R64" s="4">
+        <v>416</v>
+      </c>
+      <c r="S64" s="4">
+        <v>412</v>
+      </c>
     </row>
     <row r="65" spans="1:23">
       <c r="A65" s="11" t="s">
@@ -4101,6 +4455,12 @@
       <c r="Q65" s="4">
         <v>257</v>
       </c>
+      <c r="R65" s="4">
+        <v>294</v>
+      </c>
+      <c r="S65" s="4">
+        <v>319</v>
+      </c>
     </row>
     <row r="66" spans="1:23">
       <c r="A66" s="12" t="s">
@@ -4154,6 +4514,12 @@
       <c r="Q66" s="4">
         <v>721</v>
       </c>
+      <c r="R66" s="4">
+        <v>783</v>
+      </c>
+      <c r="S66" s="4">
+        <v>836</v>
+      </c>
     </row>
     <row r="67" spans="1:23">
       <c r="A67" s="12" t="s">
@@ -4207,6 +4573,12 @@
       <c r="Q67" s="4">
         <v>458</v>
       </c>
+      <c r="R67" s="4">
+        <v>455</v>
+      </c>
+      <c r="S67" s="4">
+        <v>487</v>
+      </c>
     </row>
     <row r="68" spans="1:23">
       <c r="A68" s="13" t="s">
@@ -4260,6 +4632,12 @@
       <c r="Q68" s="4">
         <v>81</v>
       </c>
+      <c r="R68" s="4">
+        <v>104</v>
+      </c>
+      <c r="S68" s="4">
+        <v>118</v>
+      </c>
     </row>
     <row r="69" spans="1:23">
       <c r="A69" s="13" t="s">
@@ -4313,6 +4691,12 @@
       <c r="Q69" s="4">
         <v>-19</v>
       </c>
+      <c r="R69" s="4">
+        <v>-53</v>
+      </c>
+      <c r="S69" s="4">
+        <v>-37</v>
+      </c>
     </row>
     <row r="70" spans="1:23">
       <c r="A70" s="5" t="s">
@@ -4366,6 +4750,12 @@
       <c r="Q70" s="4">
         <v>9</v>
       </c>
+      <c r="R70" s="4">
+        <v>9</v>
+      </c>
+      <c r="S70" s="4">
+        <v>10</v>
+      </c>
     </row>
     <row r="71" spans="1:23">
       <c r="A71" s="5" t="s">
@@ -4419,6 +4809,12 @@
       <c r="Q71" s="4">
         <v>37</v>
       </c>
+      <c r="R71" s="4">
+        <v>21</v>
+      </c>
+      <c r="S71" s="4">
+        <v>21</v>
+      </c>
     </row>
     <row r="73" spans="1:23">
       <c r="A73" s="1" t="s">
@@ -4543,6 +4939,12 @@
       <c r="Q74" s="4">
         <v>127.5</v>
       </c>
+      <c r="R74" s="4">
+        <v>136.7</v>
+      </c>
+      <c r="S74" s="4">
+        <v>146.4</v>
+      </c>
     </row>
     <row r="75" spans="1:23">
       <c r="A75" s="3" t="s">
@@ -4596,6 +4998,12 @@
       <c r="Q75" s="4">
         <v>83.40000000000002</v>
       </c>
+      <c r="R75" s="4">
+        <v>90.60000000000002</v>
+      </c>
+      <c r="S75" s="4">
+        <v>97.80000000000003</v>
+      </c>
     </row>
     <row r="76" spans="1:23">
       <c r="A76" s="5" t="s">
@@ -4649,6 +5057,12 @@
       <c r="Q76" s="4">
         <v>80.40000000000002</v>
       </c>
+      <c r="R76" s="4">
+        <v>86.30000000000003</v>
+      </c>
+      <c r="S76" s="4">
+        <v>93.20000000000003</v>
+      </c>
     </row>
     <row r="77" spans="1:23">
       <c r="A77" s="5" t="s">
@@ -4702,6 +5116,12 @@
       <c r="Q77" s="4">
         <v>47</v>
       </c>
+      <c r="R77" s="4">
+        <v>47</v>
+      </c>
+      <c r="S77" s="4">
+        <v>47</v>
+      </c>
     </row>
     <row r="78" spans="1:23">
       <c r="A78" s="6" t="s">
@@ -4755,6 +5175,12 @@
       <c r="Q78" s="4">
         <v>159.8</v>
       </c>
+      <c r="R78" s="4">
+        <v>171.3</v>
+      </c>
+      <c r="S78" s="4">
+        <v>182.8</v>
+      </c>
     </row>
     <row r="79" spans="1:23">
       <c r="A79" s="6" t="s">
@@ -4808,6 +5234,12 @@
       <c r="Q79" s="4">
         <v>142.7</v>
       </c>
+      <c r="R79" s="4">
+        <v>154.7</v>
+      </c>
+      <c r="S79" s="4">
+        <v>167.7</v>
+      </c>
     </row>
     <row r="80" spans="1:23">
       <c r="A80" s="7" t="s">
@@ -4861,8 +5293,14 @@
       <c r="Q80" s="4">
         <v>139.1</v>
       </c>
-    </row>
-    <row r="81" spans="1:17">
+      <c r="R80" s="4">
+        <v>150.1</v>
+      </c>
+      <c r="S80" s="4">
+        <v>161.6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19">
       <c r="A81" s="7" t="s">
         <v>32</v>
       </c>
@@ -4914,8 +5352,14 @@
       <c r="Q81" s="4">
         <v>174.3</v>
       </c>
-    </row>
-    <row r="82" spans="1:17">
+      <c r="R81" s="4">
+        <v>189.7</v>
+      </c>
+      <c r="S81" s="4">
+        <v>204.9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19">
       <c r="A82" s="8" t="s">
         <v>33</v>
       </c>
@@ -4967,8 +5411,14 @@
       <c r="Q82" s="4">
         <v>347.9</v>
       </c>
-    </row>
-    <row r="83" spans="1:17">
+      <c r="R82" s="4">
+        <v>371.2</v>
+      </c>
+      <c r="S82" s="4">
+        <v>394.3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19">
       <c r="A83" s="8" t="s">
         <v>34</v>
       </c>
@@ -5020,8 +5470,14 @@
       <c r="Q83" s="4">
         <v>275.9</v>
       </c>
-    </row>
-    <row r="84" spans="1:17">
+      <c r="R83" s="4">
+        <v>295.3</v>
+      </c>
+      <c r="S83" s="4">
+        <v>314.9999999999999</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19">
       <c r="A84" s="9" t="s">
         <v>35</v>
       </c>
@@ -5073,8 +5529,14 @@
       <c r="Q84" s="4">
         <v>112.3</v>
       </c>
-    </row>
-    <row r="85" spans="1:17">
+      <c r="R84" s="4">
+        <v>121.6</v>
+      </c>
+      <c r="S84" s="4">
+        <v>131.4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19">
       <c r="A85" s="9" t="s">
         <v>36</v>
       </c>
@@ -5126,8 +5588,14 @@
       <c r="Q85" s="4">
         <v>67.19999999999997</v>
       </c>
-    </row>
-    <row r="86" spans="1:17">
+      <c r="R85" s="4">
+        <v>72.39999999999998</v>
+      </c>
+      <c r="S85" s="4">
+        <v>78.09999999999998</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19">
       <c r="A86" s="10" t="s">
         <v>37</v>
       </c>
@@ -5179,8 +5647,14 @@
       <c r="Q86" s="4">
         <v>203.6</v>
       </c>
-    </row>
-    <row r="87" spans="1:17">
+      <c r="R86" s="4">
+        <v>220.6</v>
+      </c>
+      <c r="S86" s="4">
+        <v>238.6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19">
       <c r="A87" s="10" t="s">
         <v>38</v>
       </c>
@@ -5232,8 +5706,14 @@
       <c r="Q87" s="4">
         <v>129.6</v>
       </c>
-    </row>
-    <row r="88" spans="1:17">
+      <c r="R87" s="4">
+        <v>143.6</v>
+      </c>
+      <c r="S87" s="4">
+        <v>157.5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19">
       <c r="A88" s="11" t="s">
         <v>39</v>
       </c>
@@ -5285,8 +5765,14 @@
       <c r="Q88" s="4">
         <v>391.8000000000001</v>
       </c>
-    </row>
-    <row r="89" spans="1:17">
+      <c r="R88" s="4">
+        <v>417.1000000000001</v>
+      </c>
+      <c r="S88" s="4">
+        <v>442.1000000000001</v>
+      </c>
+    </row>
+    <row r="89" spans="1:19">
       <c r="A89" s="11" t="s">
         <v>40</v>
       </c>
@@ -5338,8 +5824,14 @@
       <c r="Q89" s="4">
         <v>301.8</v>
       </c>
-    </row>
-    <row r="90" spans="1:17">
+      <c r="R89" s="4">
+        <v>321.7</v>
+      </c>
+      <c r="S89" s="4">
+        <v>341.9</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19">
       <c r="A90" s="12" t="s">
         <v>41</v>
       </c>
@@ -5391,8 +5883,14 @@
       <c r="Q90" s="4">
         <v>447.1000000000001</v>
       </c>
-    </row>
-    <row r="91" spans="1:17">
+      <c r="R90" s="4">
+        <v>476.4000000000001</v>
+      </c>
+      <c r="S90" s="4">
+        <v>505.9000000000001</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19">
       <c r="A91" s="12" t="s">
         <v>42</v>
       </c>
@@ -5444,8 +5942,14 @@
       <c r="Q91" s="4">
         <v>307.8000000000001</v>
       </c>
-    </row>
-    <row r="92" spans="1:17">
+      <c r="R91" s="4">
+        <v>327.9000000000001</v>
+      </c>
+      <c r="S91" s="4">
+        <v>348.3000000000001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19">
       <c r="A92" s="13" t="s">
         <v>43</v>
       </c>
@@ -5497,8 +6001,14 @@
       <c r="Q92" s="4">
         <v>106.9</v>
       </c>
-    </row>
-    <row r="93" spans="1:17">
+      <c r="R92" s="4">
+        <v>117.2</v>
+      </c>
+      <c r="S92" s="4">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19">
       <c r="A93" s="13" t="s">
         <v>44</v>
       </c>
@@ -5550,8 +6060,14 @@
       <c r="Q93" s="4">
         <v>65.90000000000001</v>
       </c>
-    </row>
-    <row r="94" spans="1:17">
+      <c r="R93" s="4">
+        <v>70.7</v>
+      </c>
+      <c r="S93" s="4">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="94" spans="1:19">
       <c r="A94" s="5" t="s">
         <v>27</v>
       </c>
@@ -5603,8 +6119,14 @@
       <c r="Q94" s="4">
         <v>13.5</v>
       </c>
-    </row>
-    <row r="95" spans="1:17">
+      <c r="R94" s="4">
+        <v>18</v>
+      </c>
+      <c r="S94" s="4">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:19">
       <c r="A95" s="5" t="s">
         <v>28</v>
       </c>
@@ -5654,6 +6176,12 @@
         <v>20</v>
       </c>
       <c r="Q95" s="4">
+        <v>26</v>
+      </c>
+      <c r="R95" s="4">
+        <v>26</v>
+      </c>
+      <c r="S95" s="4">
         <v>26</v>
       </c>
     </row>
@@ -5780,6 +6308,12 @@
       <c r="Q98" s="4">
         <v>2.25</v>
       </c>
+      <c r="R98" s="4">
+        <v>3</v>
+      </c>
+      <c r="S98" s="4">
+        <v>3.388888888888889</v>
+      </c>
     </row>
     <row r="99" spans="1:23">
       <c r="A99" s="3" t="s">
@@ -5833,6 +6367,12 @@
       <c r="Q99" s="4">
         <v>6.3125</v>
       </c>
+      <c r="R99" s="4">
+        <v>7.058823529411764</v>
+      </c>
+      <c r="S99" s="4">
+        <v>6.777777777777778</v>
+      </c>
     </row>
     <row r="100" spans="1:23">
       <c r="A100" s="5" t="s">
@@ -5886,6 +6426,12 @@
       <c r="Q100" s="4">
         <v>2.625</v>
       </c>
+      <c r="R100" s="4">
+        <v>3.117647058823529</v>
+      </c>
+      <c r="S100" s="4">
+        <v>4.611111111111111</v>
+      </c>
     </row>
     <row r="101" spans="1:23">
       <c r="A101" s="5" t="s">
@@ -5939,6 +6485,12 @@
       <c r="Q101" s="4">
         <v>1.25</v>
       </c>
+      <c r="R101" s="4">
+        <v>1.176470588235294</v>
+      </c>
+      <c r="S101" s="4">
+        <v>1.111111111111111</v>
+      </c>
     </row>
     <row r="102" spans="1:23">
       <c r="A102" s="6" t="s">
@@ -5992,6 +6544,12 @@
       <c r="Q102" s="4">
         <v>3.6875</v>
       </c>
+      <c r="R102" s="4">
+        <v>3.588235294117647</v>
+      </c>
+      <c r="S102" s="4">
+        <v>2.833333333333333</v>
+      </c>
     </row>
     <row r="103" spans="1:23">
       <c r="A103" s="6" t="s">
@@ -6045,6 +6603,12 @@
       <c r="Q103" s="4">
         <v>9.875</v>
       </c>
+      <c r="R103" s="4">
+        <v>9.941176470588236</v>
+      </c>
+      <c r="S103" s="4">
+        <v>10.61111111111111</v>
+      </c>
     </row>
     <row r="104" spans="1:23">
       <c r="A104" s="7" t="s">
@@ -6098,6 +6662,12 @@
       <c r="Q104" s="4">
         <v>7.375</v>
       </c>
+      <c r="R104" s="4">
+        <v>7.941176470588236</v>
+      </c>
+      <c r="S104" s="4">
+        <v>8.055555555555555</v>
+      </c>
     </row>
     <row r="105" spans="1:23">
       <c r="A105" s="7" t="s">
@@ -6151,6 +6721,12 @@
       <c r="Q105" s="4">
         <v>21</v>
       </c>
+      <c r="R105" s="4">
+        <v>21.23529411764706</v>
+      </c>
+      <c r="S105" s="4">
+        <v>19.55555555555556</v>
+      </c>
     </row>
     <row r="106" spans="1:23">
       <c r="A106" s="8" t="s">
@@ -6204,6 +6780,12 @@
       <c r="Q106" s="4">
         <v>14.5</v>
       </c>
+      <c r="R106" s="4">
+        <v>14.94117647058824</v>
+      </c>
+      <c r="S106" s="4">
+        <v>13.55555555555556</v>
+      </c>
     </row>
     <row r="107" spans="1:23">
       <c r="A107" s="8" t="s">
@@ -6257,6 +6839,12 @@
       <c r="Q107" s="4">
         <v>18.625</v>
       </c>
+      <c r="R107" s="4">
+        <v>16.70588235294118</v>
+      </c>
+      <c r="S107" s="4">
+        <v>17.55555555555556</v>
+      </c>
     </row>
     <row r="108" spans="1:23">
       <c r="A108" s="9" t="s">
@@ -6310,6 +6898,12 @@
       <c r="Q108" s="4">
         <v>5.375</v>
       </c>
+      <c r="R108" s="4">
+        <v>6.411764705882353</v>
+      </c>
+      <c r="S108" s="4">
+        <v>6.722222222222222</v>
+      </c>
     </row>
     <row r="109" spans="1:23">
       <c r="A109" s="9" t="s">
@@ -6363,6 +6957,12 @@
       <c r="Q109" s="4">
         <v>3.375</v>
       </c>
+      <c r="R109" s="4">
+        <v>2.117647058823529</v>
+      </c>
+      <c r="S109" s="4">
+        <v>2.944444444444445</v>
+      </c>
     </row>
     <row r="110" spans="1:23">
       <c r="A110" s="10" t="s">
@@ -6416,6 +7016,12 @@
       <c r="Q110" s="4">
         <v>14.875</v>
       </c>
+      <c r="R110" s="4">
+        <v>16.41176470588235</v>
+      </c>
+      <c r="S110" s="4">
+        <v>18.05555555555556</v>
+      </c>
     </row>
     <row r="111" spans="1:23">
       <c r="A111" s="10" t="s">
@@ -6469,6 +7075,12 @@
       <c r="Q111" s="4">
         <v>10.5</v>
       </c>
+      <c r="R111" s="4">
+        <v>13.17647058823529</v>
+      </c>
+      <c r="S111" s="4">
+        <v>11.33333333333333</v>
+      </c>
     </row>
     <row r="112" spans="1:23">
       <c r="A112" s="11" t="s">
@@ -6522,6 +7134,12 @@
       <c r="Q112" s="4">
         <v>25.625</v>
       </c>
+      <c r="R112" s="4">
+        <v>24.47058823529412</v>
+      </c>
+      <c r="S112" s="4">
+        <v>22.88888888888889</v>
+      </c>
     </row>
     <row r="113" spans="1:23">
       <c r="A113" s="11" t="s">
@@ -6575,6 +7193,12 @@
       <c r="Q113" s="4">
         <v>16.0625</v>
       </c>
+      <c r="R113" s="4">
+        <v>17.29411764705882</v>
+      </c>
+      <c r="S113" s="4">
+        <v>17.72222222222222</v>
+      </c>
     </row>
     <row r="114" spans="1:23">
       <c r="A114" s="12" t="s">
@@ -6628,6 +7252,12 @@
       <c r="Q114" s="4">
         <v>45.0625</v>
       </c>
+      <c r="R114" s="4">
+        <v>46.05882352941177</v>
+      </c>
+      <c r="S114" s="4">
+        <v>46.44444444444444</v>
+      </c>
     </row>
     <row r="115" spans="1:23">
       <c r="A115" s="12" t="s">
@@ -6681,6 +7311,12 @@
       <c r="Q115" s="4">
         <v>28.625</v>
       </c>
+      <c r="R115" s="4">
+        <v>26.76470588235294</v>
+      </c>
+      <c r="S115" s="4">
+        <v>27.05555555555556</v>
+      </c>
     </row>
     <row r="116" spans="1:23">
       <c r="A116" s="13" t="s">
@@ -6734,6 +7370,12 @@
       <c r="Q116" s="4">
         <v>5.0625</v>
       </c>
+      <c r="R116" s="4">
+        <v>6.117647058823529</v>
+      </c>
+      <c r="S116" s="4">
+        <v>6.555555555555555</v>
+      </c>
     </row>
     <row r="117" spans="1:23">
       <c r="A117" s="13" t="s">
@@ -6787,6 +7429,12 @@
       <c r="Q117" s="4">
         <v>-1.1875</v>
       </c>
+      <c r="R117" s="4">
+        <v>-3.117647058823529</v>
+      </c>
+      <c r="S117" s="4">
+        <v>-2.055555555555555</v>
+      </c>
     </row>
     <row r="118" spans="1:23">
       <c r="A118" s="5" t="s">
@@ -6840,6 +7488,12 @@
       <c r="Q118" s="4">
         <v>0.5625</v>
       </c>
+      <c r="R118" s="4">
+        <v>0.5294117647058824</v>
+      </c>
+      <c r="S118" s="4">
+        <v>0.5555555555555556</v>
+      </c>
     </row>
     <row r="119" spans="1:23">
       <c r="A119" s="5" t="s">
@@ -6893,6 +7547,12 @@
       <c r="Q119" s="4">
         <v>2.3125</v>
       </c>
+      <c r="R119" s="4">
+        <v>1.235294117647059</v>
+      </c>
+      <c r="S119" s="4">
+        <v>1.166666666666667</v>
+      </c>
     </row>
     <row r="121" spans="1:23">
       <c r="A121" s="1" t="s">
@@ -7017,6 +7677,12 @@
       <c r="Q122" s="4">
         <v>7.968750000000002</v>
       </c>
+      <c r="R122" s="4">
+        <v>8.041176470588237</v>
+      </c>
+      <c r="S122" s="4">
+        <v>8.133333333333333</v>
+      </c>
     </row>
     <row r="123" spans="1:23">
       <c r="A123" s="3" t="s">
@@ -7070,6 +7736,12 @@
       <c r="Q123" s="4">
         <v>5.212500000000001</v>
       </c>
+      <c r="R123" s="4">
+        <v>5.329411764705884</v>
+      </c>
+      <c r="S123" s="4">
+        <v>5.433333333333334</v>
+      </c>
     </row>
     <row r="124" spans="1:23">
       <c r="A124" s="5" t="s">
@@ -7123,6 +7795,12 @@
       <c r="Q124" s="4">
         <v>5.025000000000001</v>
       </c>
+      <c r="R124" s="4">
+        <v>5.076470588235296</v>
+      </c>
+      <c r="S124" s="4">
+        <v>5.17777777777778</v>
+      </c>
     </row>
     <row r="125" spans="1:23">
       <c r="A125" s="5" t="s">
@@ -7176,6 +7854,12 @@
       <c r="Q125" s="4">
         <v>2.9375</v>
       </c>
+      <c r="R125" s="4">
+        <v>2.764705882352941</v>
+      </c>
+      <c r="S125" s="4">
+        <v>2.611111111111111</v>
+      </c>
     </row>
     <row r="126" spans="1:23">
       <c r="A126" s="6" t="s">
@@ -7229,6 +7913,12 @@
       <c r="Q126" s="4">
         <v>9.987500000000001</v>
       </c>
+      <c r="R126" s="4">
+        <v>10.0764705882353</v>
+      </c>
+      <c r="S126" s="4">
+        <v>10.15555555555556</v>
+      </c>
     </row>
     <row r="127" spans="1:23">
       <c r="A127" s="6" t="s">
@@ -7282,6 +7972,12 @@
       <c r="Q127" s="4">
         <v>8.918749999999999</v>
       </c>
+      <c r="R127" s="4">
+        <v>9.1</v>
+      </c>
+      <c r="S127" s="4">
+        <v>9.316666666666666</v>
+      </c>
     </row>
     <row r="128" spans="1:23">
       <c r="A128" s="7" t="s">
@@ -7335,8 +8031,14 @@
       <c r="Q128" s="4">
         <v>8.693749999999998</v>
       </c>
-    </row>
-    <row r="129" spans="1:17">
+      <c r="R128" s="4">
+        <v>8.829411764705881</v>
+      </c>
+      <c r="S128" s="4">
+        <v>8.977777777777776</v>
+      </c>
+    </row>
+    <row r="129" spans="1:19">
       <c r="A129" s="7" t="s">
         <v>32</v>
       </c>
@@ -7388,8 +8090,14 @@
       <c r="Q129" s="4">
         <v>10.89375</v>
       </c>
-    </row>
-    <row r="130" spans="1:17">
+      <c r="R129" s="4">
+        <v>11.15882352941177</v>
+      </c>
+      <c r="S129" s="4">
+        <v>11.38333333333333</v>
+      </c>
+    </row>
+    <row r="130" spans="1:19">
       <c r="A130" s="8" t="s">
         <v>33</v>
       </c>
@@ -7441,8 +8149,14 @@
       <c r="Q130" s="4">
         <v>21.74375</v>
       </c>
-    </row>
-    <row r="131" spans="1:17">
+      <c r="R130" s="4">
+        <v>21.83529411764706</v>
+      </c>
+      <c r="S130" s="4">
+        <v>21.90555555555556</v>
+      </c>
+    </row>
+    <row r="131" spans="1:19">
       <c r="A131" s="8" t="s">
         <v>34</v>
       </c>
@@ -7494,8 +8208,14 @@
       <c r="Q131" s="4">
         <v>17.24375</v>
       </c>
-    </row>
-    <row r="132" spans="1:17">
+      <c r="R131" s="4">
+        <v>17.37058823529411</v>
+      </c>
+      <c r="S131" s="4">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="132" spans="1:19">
       <c r="A132" s="9" t="s">
         <v>35</v>
       </c>
@@ -7547,8 +8267,14 @@
       <c r="Q132" s="4">
         <v>7.018749999999999</v>
       </c>
-    </row>
-    <row r="133" spans="1:17">
+      <c r="R132" s="4">
+        <v>7.152941176470587</v>
+      </c>
+      <c r="S132" s="4">
+        <v>7.299999999999999</v>
+      </c>
+    </row>
+    <row r="133" spans="1:19">
       <c r="A133" s="9" t="s">
         <v>36</v>
       </c>
@@ -7600,8 +8326,14 @@
       <c r="Q133" s="4">
         <v>4.199999999999998</v>
       </c>
-    </row>
-    <row r="134" spans="1:17">
+      <c r="R133" s="4">
+        <v>4.258823529411764</v>
+      </c>
+      <c r="S133" s="4">
+        <v>4.338888888888888</v>
+      </c>
+    </row>
+    <row r="134" spans="1:19">
       <c r="A134" s="10" t="s">
         <v>37</v>
       </c>
@@ -7653,8 +8385,14 @@
       <c r="Q134" s="4">
         <v>12.725</v>
       </c>
-    </row>
-    <row r="135" spans="1:17">
+      <c r="R134" s="4">
+        <v>12.9764705882353</v>
+      </c>
+      <c r="S134" s="4">
+        <v>13.25555555555556</v>
+      </c>
+    </row>
+    <row r="135" spans="1:19">
       <c r="A135" s="10" t="s">
         <v>38</v>
       </c>
@@ -7706,8 +8444,14 @@
       <c r="Q135" s="4">
         <v>8.1</v>
       </c>
-    </row>
-    <row r="136" spans="1:17">
+      <c r="R135" s="4">
+        <v>8.447058823529412</v>
+      </c>
+      <c r="S135" s="4">
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="136" spans="1:19">
       <c r="A136" s="11" t="s">
         <v>39</v>
       </c>
@@ -7759,8 +8503,14 @@
       <c r="Q136" s="4">
         <v>24.4875</v>
       </c>
-    </row>
-    <row r="137" spans="1:17">
+      <c r="R136" s="4">
+        <v>24.53529411764706</v>
+      </c>
+      <c r="S136" s="4">
+        <v>24.56111111111112</v>
+      </c>
+    </row>
+    <row r="137" spans="1:19">
       <c r="A137" s="11" t="s">
         <v>40</v>
       </c>
@@ -7812,8 +8562,14 @@
       <c r="Q137" s="4">
         <v>18.8625</v>
       </c>
-    </row>
-    <row r="138" spans="1:17">
+      <c r="R137" s="4">
+        <v>18.9235294117647</v>
+      </c>
+      <c r="S137" s="4">
+        <v>18.99444444444444</v>
+      </c>
+    </row>
+    <row r="138" spans="1:19">
       <c r="A138" s="12" t="s">
         <v>41</v>
       </c>
@@ -7865,8 +8621,14 @@
       <c r="Q138" s="4">
         <v>27.94375</v>
       </c>
-    </row>
-    <row r="139" spans="1:17">
+      <c r="R138" s="4">
+        <v>28.02352941176471</v>
+      </c>
+      <c r="S138" s="4">
+        <v>28.10555555555556</v>
+      </c>
+    </row>
+    <row r="139" spans="1:19">
       <c r="A139" s="12" t="s">
         <v>42</v>
       </c>
@@ -7918,8 +8680,14 @@
       <c r="Q139" s="4">
         <v>19.2375</v>
       </c>
-    </row>
-    <row r="140" spans="1:17">
+      <c r="R139" s="4">
+        <v>19.28823529411765</v>
+      </c>
+      <c r="S139" s="4">
+        <v>19.35</v>
+      </c>
+    </row>
+    <row r="140" spans="1:19">
       <c r="A140" s="13" t="s">
         <v>43</v>
       </c>
@@ -7971,8 +8739,14 @@
       <c r="Q140" s="4">
         <v>6.68125</v>
       </c>
-    </row>
-    <row r="141" spans="1:17">
+      <c r="R140" s="4">
+        <v>6.894117647058824</v>
+      </c>
+      <c r="S140" s="4">
+        <v>7.111111111111111</v>
+      </c>
+    </row>
+    <row r="141" spans="1:19">
       <c r="A141" s="13" t="s">
         <v>44</v>
       </c>
@@ -8024,8 +8798,14 @@
       <c r="Q141" s="4">
         <v>4.11875</v>
       </c>
-    </row>
-    <row r="142" spans="1:17">
+      <c r="R141" s="4">
+        <v>4.158823529411765</v>
+      </c>
+      <c r="S141" s="4">
+        <v>4.222222222222222</v>
+      </c>
+    </row>
+    <row r="142" spans="1:19">
       <c r="A142" s="5" t="s">
         <v>27</v>
       </c>
@@ -8077,8 +8857,14 @@
       <c r="Q142" s="4">
         <v>0.84375</v>
       </c>
-    </row>
-    <row r="143" spans="1:17">
+      <c r="R142" s="4">
+        <v>1.058823529411765</v>
+      </c>
+      <c r="S142" s="4">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="143" spans="1:19">
       <c r="A143" s="5" t="s">
         <v>28</v>
       </c>
@@ -8129,6 +8915,12 @@
       </c>
       <c r="Q143" s="4">
         <v>1.625</v>
+      </c>
+      <c r="R143" s="4">
+        <v>1.529411764705882</v>
+      </c>
+      <c r="S143" s="4">
+        <v>1.444444444444444</v>
       </c>
     </row>
     <row r="145" spans="1:23">
@@ -8254,6 +9046,12 @@
       <c r="Q146" s="4">
         <v>-1.931818181818182</v>
       </c>
+      <c r="R146" s="4">
+        <v>1.724137931034483</v>
+      </c>
+      <c r="S146" s="4">
+        <v>1.086956521739131</v>
+      </c>
     </row>
     <row r="147" spans="1:23">
       <c r="A147" s="3" t="s">
@@ -8307,6 +9105,12 @@
       <c r="Q147" s="4">
         <v>1.290322580645161</v>
       </c>
+      <c r="R147" s="4">
+        <v>2.835820895522388</v>
+      </c>
+      <c r="S147" s="4">
+        <v>0.2777777777777778</v>
+      </c>
     </row>
     <row r="148" spans="1:23">
       <c r="A148" s="5" t="s">
@@ -8360,6 +9164,12 @@
       <c r="Q148" s="4">
         <v>0.3703703703703703</v>
       </c>
+      <c r="R148" s="4">
+        <v>2.037037037037037</v>
+      </c>
+      <c r="S148" s="4">
+        <v>5.084745762711864</v>
+      </c>
     </row>
     <row r="149" spans="1:23">
       <c r="A149" s="5" t="s">
@@ -8413,6 +9223,12 @@
       <c r="Q149" s="4">
         <v>0</v>
       </c>
+      <c r="R149" s="4">
+        <v>0</v>
+      </c>
+      <c r="S149" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="150" spans="1:23">
       <c r="A150" s="6" t="s">
@@ -8466,6 +9282,12 @@
       <c r="Q150" s="4">
         <v>0.9090909090909091</v>
       </c>
+      <c r="R150" s="4">
+        <v>0.1739130434782609</v>
+      </c>
+      <c r="S150" s="4">
+        <v>-0.8695652173913043</v>
+      </c>
     </row>
     <row r="151" spans="1:23">
       <c r="A151" s="6" t="s">
@@ -8519,6 +9341,12 @@
       <c r="Q151" s="4">
         <v>0.6363636363636364</v>
       </c>
+      <c r="R151" s="4">
+        <v>0.9565217391304348</v>
+      </c>
+      <c r="S151" s="4">
+        <v>1.833333333333333</v>
+      </c>
     </row>
     <row r="152" spans="1:23">
       <c r="A152" s="7" t="s">
@@ -8572,6 +9400,12 @@
       <c r="Q152" s="4">
         <v>-1.320754716981132</v>
       </c>
+      <c r="R152" s="4">
+        <v>1.619047619047619</v>
+      </c>
+      <c r="S152" s="4">
+        <v>0.9090909090909091</v>
+      </c>
     </row>
     <row r="153" spans="1:23">
       <c r="A153" s="7" t="s">
@@ -8625,6 +9459,12 @@
       <c r="Q153" s="4">
         <v>1.194029850746269</v>
       </c>
+      <c r="R153" s="4">
+        <v>1.736111111111111</v>
+      </c>
+      <c r="S153" s="4">
+        <v>-0.5844155844155844</v>
+      </c>
     </row>
     <row r="154" spans="1:23">
       <c r="A154" s="8" t="s">
@@ -8678,6 +9518,12 @@
       <c r="Q154" s="4">
         <v>0.9691629955947136</v>
       </c>
+      <c r="R154" s="4">
+        <v>0.9565217391304348</v>
+      </c>
+      <c r="S154" s="4">
+        <v>-0.4291845493562232</v>
+      </c>
     </row>
     <row r="155" spans="1:23">
       <c r="A155" s="8" t="s">
@@ -8731,6 +9577,12 @@
       <c r="Q155" s="4">
         <v>0.9183673469387754</v>
       </c>
+      <c r="R155" s="4">
+        <v>-0.7035175879396985</v>
+      </c>
+      <c r="S155" s="4">
+        <v>1.649484536082474</v>
+      </c>
     </row>
     <row r="156" spans="1:23">
       <c r="A156" s="9" t="s">
@@ -8784,6 +9636,12 @@
       <c r="Q156" s="4">
         <v>0.4819277108433734</v>
       </c>
+      <c r="R156" s="4">
+        <v>2.771084337349397</v>
+      </c>
+      <c r="S156" s="4">
+        <v>1.290322580645161</v>
+      </c>
     </row>
     <row r="157" spans="1:23">
       <c r="A157" s="9" t="s">
@@ -8837,6 +9695,12 @@
       <c r="Q157" s="4">
         <v>2.083333333333333</v>
       </c>
+      <c r="R157" s="4">
+        <v>-3.39622641509434</v>
+      </c>
+      <c r="S157" s="4">
+        <v>3.269230769230769</v>
+      </c>
     </row>
     <row r="158" spans="1:23">
       <c r="A158" s="10" t="s">
@@ -8890,6 +9754,12 @@
       <c r="Q158" s="4">
         <v>1.974522292993631</v>
       </c>
+      <c r="R158" s="4">
+        <v>2.455089820359281</v>
+      </c>
+      <c r="S158" s="4">
+        <v>2.705882352941177</v>
+      </c>
     </row>
     <row r="159" spans="1:23">
       <c r="A159" s="10" t="s">
@@ -8943,6 +9813,12 @@
       <c r="Q159" s="4">
         <v>3.181818181818182</v>
       </c>
+      <c r="R159" s="4">
+        <v>4.48</v>
+      </c>
+      <c r="S159" s="4">
+        <v>-1.428571428571429</v>
+      </c>
     </row>
     <row r="160" spans="1:23">
       <c r="A160" s="11" t="s">
@@ -8996,6 +9872,12 @@
       <c r="Q160" s="4">
         <v>0.7843137254901961</v>
       </c>
+      <c r="R160" s="4">
+        <v>0.234375</v>
+      </c>
+      <c r="S160" s="4">
+        <v>-0.158102766798419</v>
+      </c>
     </row>
     <row r="161" spans="1:23">
       <c r="A161" s="11" t="s">
@@ -9049,6 +9931,12 @@
       <c r="Q161" s="4">
         <v>0.7253886010362695</v>
       </c>
+      <c r="R161" s="4">
+        <v>1.887755102040816</v>
+      </c>
+      <c r="S161" s="4">
+        <v>1.256281407035176</v>
+      </c>
     </row>
     <row r="162" spans="1:23">
       <c r="A162" s="12" t="s">
@@ -9102,6 +9990,12 @@
       <c r="Q162" s="4">
         <v>1.626297577854671</v>
       </c>
+      <c r="R162" s="4">
+        <v>2.130584192439863</v>
+      </c>
+      <c r="S162" s="4">
+        <v>1.808873720136519</v>
+      </c>
     </row>
     <row r="163" spans="1:23">
       <c r="A163" s="12" t="s">
@@ -9155,6 +10049,12 @@
       <c r="Q163" s="4">
         <v>-0.5288461538461539</v>
       </c>
+      <c r="R163" s="4">
+        <v>-0.1477832512315271</v>
+      </c>
+      <c r="S163" s="4">
+        <v>1.592039800995025</v>
+      </c>
     </row>
     <row r="164" spans="1:23">
       <c r="A164" s="13" t="s">
@@ -9208,6 +10108,12 @@
       <c r="Q164" s="4">
         <v>-1.595744680851064</v>
       </c>
+      <c r="R164" s="4">
+        <v>2.473118279569892</v>
+      </c>
+      <c r="S164" s="4">
+        <v>1.359223300970874</v>
+      </c>
     </row>
     <row r="165" spans="1:23">
       <c r="A165" s="13" t="s">
@@ -9261,6 +10167,12 @@
       <c r="Q165" s="4">
         <v>-4.2</v>
       </c>
+      <c r="R165" s="4">
+        <v>-6.938775510204081</v>
+      </c>
+      <c r="S165" s="4">
+        <v>3.333333333333333</v>
+      </c>
     </row>
     <row r="166" spans="1:23">
       <c r="A166" s="5" t="s">
@@ -9314,6 +10226,12 @@
       <c r="Q166" s="4">
         <v>0</v>
       </c>
+      <c r="R166" s="4">
+        <v>0</v>
+      </c>
+      <c r="S166" s="4">
+        <v>0.2222222222222222</v>
+      </c>
     </row>
     <row r="167" spans="1:23">
       <c r="A167" s="5" t="s">
@@ -9367,6 +10285,12 @@
       <c r="Q167" s="4">
         <v>0.9090909090909091</v>
       </c>
+      <c r="R167" s="4">
+        <v>-2.666666666666667</v>
+      </c>
+      <c r="S167" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="169" spans="1:23">
       <c r="A169" s="1" t="s">
@@ -9491,6 +10415,12 @@
       <c r="Q170" s="4">
         <v>0.3032855939342881</v>
       </c>
+      <c r="R170" s="4">
+        <v>0.4003139717425431</v>
+      </c>
+      <c r="S170" s="4">
+        <v>0.4465592972181551</v>
+      </c>
     </row>
     <row r="171" spans="1:23">
       <c r="A171" s="3" t="s">
@@ -9544,6 +10474,12 @@
       <c r="Q171" s="4">
         <v>1.237745098039215</v>
       </c>
+      <c r="R171" s="4">
+        <v>1.359003397508493</v>
+      </c>
+      <c r="S171" s="4">
+        <v>1.277486910994764</v>
+      </c>
     </row>
     <row r="172" spans="1:23">
       <c r="A172" s="5" t="s">
@@ -9597,6 +10533,12 @@
       <c r="Q172" s="4">
         <v>0.5263157894736842</v>
       </c>
+      <c r="R172" s="4">
+        <v>0.6220657276995304</v>
+      </c>
+      <c r="S172" s="4">
+        <v>0.9110867178924257</v>
+      </c>
     </row>
     <row r="173" spans="1:23">
       <c r="A173" s="5" t="s">
@@ -9650,6 +10592,12 @@
       <c r="Q173" s="4">
         <v>0.5263157894736842</v>
       </c>
+      <c r="R173" s="4">
+        <v>0.5263157894736842</v>
+      </c>
+      <c r="S173" s="4">
+        <v>0.5263157894736842</v>
+      </c>
     </row>
     <row r="174" spans="1:23">
       <c r="A174" s="6" t="s">
@@ -9703,6 +10651,12 @@
       <c r="Q174" s="4">
         <v>0.3743654822335025</v>
       </c>
+      <c r="R174" s="4">
+        <v>0.3607332939089296</v>
+      </c>
+      <c r="S174" s="4">
+        <v>0.2823920265780731</v>
+      </c>
     </row>
     <row r="175" spans="1:23">
       <c r="A175" s="6" t="s">
@@ -9756,6 +10710,12 @@
       <c r="Q175" s="4">
         <v>1.133428981348637</v>
       </c>
+      <c r="R175" s="4">
+        <v>1.119946984758118</v>
+      </c>
+      <c r="S175" s="4">
+        <v>1.172498465316145</v>
+      </c>
     </row>
     <row r="176" spans="1:23">
       <c r="A176" s="7" t="s">
@@ -9809,8 +10769,14 @@
       <c r="Q176" s="4">
         <v>0.9394904458598728</v>
       </c>
-    </row>
-    <row r="177" spans="1:17">
+      <c r="R176" s="4">
+        <v>0.9919177075679649</v>
+      </c>
+      <c r="S176" s="4">
+        <v>0.9857239972807617</v>
+      </c>
+    </row>
+    <row r="177" spans="1:19">
       <c r="A177" s="7" t="s">
         <v>32</v>
       </c>
@@ -9862,8 +10828,14 @@
       <c r="Q177" s="4">
         <v>1.995249406175772</v>
       </c>
-    </row>
-    <row r="178" spans="1:17">
+      <c r="R177" s="4">
+        <v>1.974835886214442</v>
+      </c>
+      <c r="S177" s="4">
+        <v>1.77598385469223</v>
+      </c>
+    </row>
+    <row r="178" spans="1:19">
       <c r="A178" s="8" t="s">
         <v>33</v>
       </c>
@@ -9915,8 +10887,14 @@
       <c r="Q178" s="4">
         <v>0.6705202312138728</v>
       </c>
-    </row>
-    <row r="179" spans="1:17">
+      <c r="R178" s="4">
+        <v>0.6883468834688347</v>
+      </c>
+      <c r="S178" s="4">
+        <v>0.6219729798623502</v>
+      </c>
+    </row>
+    <row r="179" spans="1:19">
       <c r="A179" s="8" t="s">
         <v>34</v>
       </c>
@@ -9968,8 +10946,14 @@
       <c r="Q179" s="4">
         <v>1.090775988286969</v>
       </c>
-    </row>
-    <row r="180" spans="1:17">
+      <c r="R179" s="4">
+        <v>0.9689525759126579</v>
+      </c>
+      <c r="S179" s="4">
+        <v>1.0112</v>
+      </c>
+    </row>
+    <row r="180" spans="1:19">
       <c r="A180" s="9" t="s">
         <v>35</v>
       </c>
@@ -10021,8 +11005,14 @@
       <c r="Q180" s="4">
         <v>0.8245445829338448</v>
       </c>
-    </row>
-    <row r="181" spans="1:17">
+      <c r="R180" s="4">
+        <v>0.9680284191829487</v>
+      </c>
+      <c r="S180" s="4">
+        <v>0.9926168990976212</v>
+      </c>
+    </row>
+    <row r="181" spans="1:19">
       <c r="A181" s="9" t="s">
         <v>36</v>
       </c>
@@ -10074,8 +11064,14 @@
       <c r="Q181" s="4">
         <v>1.005586592178771</v>
       </c>
-    </row>
-    <row r="182" spans="1:17">
+      <c r="R181" s="4">
+        <v>0.610169491525424</v>
+      </c>
+      <c r="S181" s="4">
+        <v>0.8255451713395642</v>
+      </c>
+    </row>
+    <row r="182" spans="1:19">
       <c r="A182" s="10" t="s">
         <v>37</v>
       </c>
@@ -10127,8 +11123,14 @@
       <c r="Q182" s="4">
         <v>1.274089935760171</v>
       </c>
-    </row>
-    <row r="183" spans="1:17">
+      <c r="R182" s="4">
+        <v>1.371007371007371</v>
+      </c>
+      <c r="S182" s="4">
+        <v>1.473922902494331</v>
+      </c>
+    </row>
+    <row r="183" spans="1:19">
       <c r="A183" s="10" t="s">
         <v>38</v>
       </c>
@@ -10180,8 +11182,14 @@
       <c r="Q183" s="4">
         <v>1.354838709677419</v>
       </c>
-    </row>
-    <row r="184" spans="1:17">
+      <c r="R183" s="4">
+        <v>1.641025641025641</v>
+      </c>
+      <c r="S183" s="4">
+        <v>1.355481727574751</v>
+      </c>
+    </row>
+    <row r="184" spans="1:19">
       <c r="A184" s="11" t="s">
         <v>39</v>
       </c>
@@ -10233,8 +11241,14 @@
       <c r="Q184" s="4">
         <v>1.051551679917928</v>
       </c>
-    </row>
-    <row r="185" spans="1:17">
+      <c r="R184" s="4">
+        <v>1.001203369434416</v>
+      </c>
+      <c r="S184" s="4">
+        <v>0.9346642468239563</v>
+      </c>
+    </row>
+    <row r="185" spans="1:19">
       <c r="A185" s="11" t="s">
         <v>40</v>
       </c>
@@ -10286,8 +11300,14 @@
       <c r="Q185" s="4">
         <v>0.8543882978723404</v>
       </c>
-    </row>
-    <row r="186" spans="1:17">
+      <c r="R185" s="4">
+        <v>0.9176029962546816</v>
+      </c>
+      <c r="S185" s="4">
+        <v>0.9374081692624154</v>
+      </c>
+    </row>
+    <row r="186" spans="1:19">
       <c r="A186" s="12" t="s">
         <v>41</v>
       </c>
@@ -10339,8 +11359,14 @@
       <c r="Q186" s="4">
         <v>1.620224719101123</v>
       </c>
-    </row>
-    <row r="187" spans="1:17">
+      <c r="R186" s="4">
+        <v>1.651550305842649</v>
+      </c>
+      <c r="S186" s="4">
+        <v>1.660707191100516</v>
+      </c>
+    </row>
+    <row r="187" spans="1:19">
       <c r="A187" s="12" t="s">
         <v>42</v>
       </c>
@@ -10392,8 +11418,14 @@
       <c r="Q187" s="4">
         <v>1.49869109947644</v>
       </c>
-    </row>
-    <row r="188" spans="1:17">
+      <c r="R187" s="4">
+        <v>1.396133783369131</v>
+      </c>
+      <c r="S187" s="4">
+        <v>1.407514450867052</v>
+      </c>
+    </row>
+    <row r="188" spans="1:19">
       <c r="A188" s="13" t="s">
         <v>43</v>
       </c>
@@ -10445,8 +11477,14 @@
       <c r="Q188" s="4">
         <v>0.8265306122448979</v>
       </c>
-    </row>
-    <row r="189" spans="1:17">
+      <c r="R188" s="4">
+        <v>0.9692451071761415</v>
+      </c>
+      <c r="S188" s="4">
+        <v>1.003401360544218</v>
+      </c>
+    </row>
+    <row r="189" spans="1:19">
       <c r="A189" s="13" t="s">
         <v>44</v>
       </c>
@@ -10498,8 +11536,14 @@
       <c r="Q189" s="4">
         <v>-0.3094462540716613</v>
       </c>
-    </row>
-    <row r="190" spans="1:17">
+      <c r="R189" s="4">
+        <v>-0.799396681749623</v>
+      </c>
+      <c r="S189" s="4">
+        <v>-0.5203938115330521</v>
+      </c>
+    </row>
+    <row r="190" spans="1:19">
       <c r="A190" s="5" t="s">
         <v>27</v>
       </c>
@@ -10551,8 +11595,14 @@
       <c r="Q190" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="191" spans="1:17">
+      <c r="R190" s="4">
+        <v>1</v>
+      </c>
+      <c r="S190" s="4">
+        <v>0.7407407407407407</v>
+      </c>
+    </row>
+    <row r="191" spans="1:19">
       <c r="A191" s="5" t="s">
         <v>28</v>
       </c>
@@ -10603,6 +11653,12 @@
       </c>
       <c r="Q191" s="4">
         <v>1.85</v>
+      </c>
+      <c r="R191" s="4">
+        <v>0.8076923076923077</v>
+      </c>
+      <c r="S191" s="4">
+        <v>0.8076923076923077</v>
       </c>
     </row>
   </sheetData>
@@ -10741,6 +11797,12 @@
       <c r="Q2" s="4">
         <v>-10</v>
       </c>
+      <c r="R2" s="4">
+        <v>39</v>
+      </c>
+      <c r="S2" s="4">
+        <v>15</v>
+      </c>
     </row>
     <row r="3" spans="1:23">
       <c r="A3" s="5" t="s">
@@ -10794,6 +11856,12 @@
       <c r="Q3" s="4">
         <v>15</v>
       </c>
+      <c r="R3" s="4">
+        <v>-4</v>
+      </c>
+      <c r="S3" s="4">
+        <v>34</v>
+      </c>
     </row>
     <row r="4" spans="1:23">
       <c r="A4" s="6" t="s">
@@ -10847,6 +11915,12 @@
       <c r="Q4" s="4">
         <v>20</v>
       </c>
+      <c r="R4" s="4">
+        <v>23</v>
+      </c>
+      <c r="S4" s="4">
+        <v>27</v>
+      </c>
     </row>
     <row r="5" spans="1:23">
       <c r="A5" s="7" t="s">
@@ -10900,6 +11974,12 @@
       <c r="Q5" s="4">
         <v>7</v>
       </c>
+      <c r="R5" s="4">
+        <v>47</v>
+      </c>
+      <c r="S5" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:23">
       <c r="A6" s="8" t="s">
@@ -10953,6 +12033,12 @@
       <c r="Q6" s="4">
         <v>65</v>
       </c>
+      <c r="R6" s="4">
+        <v>18</v>
+      </c>
+      <c r="S6" s="4">
+        <v>35</v>
+      </c>
     </row>
     <row r="7" spans="1:23">
       <c r="A7" s="9" t="s">
@@ -11006,6 +12092,12 @@
       <c r="Q7" s="4">
         <v>15</v>
       </c>
+      <c r="R7" s="4">
+        <v>6</v>
+      </c>
+      <c r="S7" s="4">
+        <v>30</v>
+      </c>
     </row>
     <row r="8" spans="1:23">
       <c r="A8" s="10" t="s">
@@ -11059,6 +12151,12 @@
       <c r="Q8" s="4">
         <v>66</v>
       </c>
+      <c r="R8" s="4">
+        <v>110</v>
+      </c>
+      <c r="S8" s="4">
+        <v>36</v>
+      </c>
     </row>
     <row r="9" spans="1:23">
       <c r="A9" s="11" t="s">
@@ -11112,6 +12210,12 @@
       <c r="Q9" s="4">
         <v>44</v>
       </c>
+      <c r="R9" s="4">
+        <v>53</v>
+      </c>
+      <c r="S9" s="4">
+        <v>31</v>
+      </c>
     </row>
     <row r="10" spans="1:23">
       <c r="A10" s="12" t="s">
@@ -11165,6 +12269,12 @@
       <c r="Q10" s="4">
         <v>46</v>
       </c>
+      <c r="R10" s="4">
+        <v>64</v>
+      </c>
+      <c r="S10" s="4">
+        <v>95</v>
+      </c>
     </row>
     <row r="11" spans="1:23">
       <c r="A11" s="13" t="s">
@@ -11218,6 +12328,12 @@
       <c r="Q11" s="4">
         <v>-35</v>
       </c>
+      <c r="R11" s="4">
+        <v>-10</v>
+      </c>
+      <c r="S11" s="4">
+        <v>29</v>
+      </c>
     </row>
     <row r="13" spans="1:23">
       <c r="A13" s="1" t="s">
@@ -11342,6 +12458,12 @@
       <c r="Q14" s="4">
         <v>6.2</v>
       </c>
+      <c r="R14" s="4">
+        <v>6.7</v>
+      </c>
+      <c r="S14" s="4">
+        <v>6.7</v>
+      </c>
     </row>
     <row r="15" spans="1:23">
       <c r="A15" s="5" t="s">
@@ -11395,6 +12517,12 @@
       <c r="Q15" s="4">
         <v>6.8</v>
       </c>
+      <c r="R15" s="4">
+        <v>6.7</v>
+      </c>
+      <c r="S15" s="4">
+        <v>7.2</v>
+      </c>
     </row>
     <row r="16" spans="1:23">
       <c r="A16" s="6" t="s">
@@ -11448,6 +12576,12 @@
       <c r="Q16" s="4">
         <v>11.7</v>
       </c>
+      <c r="R16" s="4">
+        <v>12.2</v>
+      </c>
+      <c r="S16" s="4">
+        <v>12.7</v>
+      </c>
     </row>
     <row r="17" spans="1:23">
       <c r="A17" s="7" t="s">
@@ -11501,6 +12635,12 @@
       <c r="Q17" s="4">
         <v>11.5</v>
       </c>
+      <c r="R17" s="4">
+        <v>12</v>
+      </c>
+      <c r="S17" s="4">
+        <v>12</v>
+      </c>
     </row>
     <row r="18" spans="1:23">
       <c r="A18" s="8" t="s">
@@ -11554,6 +12694,12 @@
       <c r="Q18" s="4">
         <v>24.1</v>
       </c>
+      <c r="R18" s="4">
+        <v>24.2</v>
+      </c>
+      <c r="S18" s="4">
+        <v>24.3</v>
+      </c>
     </row>
     <row r="19" spans="1:23">
       <c r="A19" s="9" t="s">
@@ -11607,6 +12753,12 @@
       <c r="Q19" s="4">
         <v>6.9</v>
       </c>
+      <c r="R19" s="4">
+        <v>6.9</v>
+      </c>
+      <c r="S19" s="4">
+        <v>7.4</v>
+      </c>
     </row>
     <row r="20" spans="1:23">
       <c r="A20" s="10" t="s">
@@ -11660,6 +12812,12 @@
       <c r="Q20" s="4">
         <v>15.3</v>
       </c>
+      <c r="R20" s="4">
+        <v>16.3</v>
+      </c>
+      <c r="S20" s="4">
+        <v>16.4</v>
+      </c>
     </row>
     <row r="21" spans="1:23">
       <c r="A21" s="11" t="s">
@@ -11713,6 +12871,12 @@
       <c r="Q21" s="4">
         <v>25.8</v>
       </c>
+      <c r="R21" s="4">
+        <v>25.9</v>
+      </c>
+      <c r="S21" s="4">
+        <v>25.9</v>
+      </c>
     </row>
     <row r="22" spans="1:23">
       <c r="A22" s="12" t="s">
@@ -11766,6 +12930,12 @@
       <c r="Q22" s="4">
         <v>29.2</v>
       </c>
+      <c r="R22" s="4">
+        <v>29.3</v>
+      </c>
+      <c r="S22" s="4">
+        <v>29.4</v>
+      </c>
     </row>
     <row r="23" spans="1:23">
       <c r="A23" s="13" t="s">
@@ -11819,6 +12989,12 @@
       <c r="Q23" s="4">
         <v>6.9</v>
       </c>
+      <c r="R23" s="4">
+        <v>6.8</v>
+      </c>
+      <c r="S23" s="4">
+        <v>7.3</v>
+      </c>
     </row>
     <row r="25" spans="1:23">
       <c r="A25" s="1" t="s">
@@ -11943,6 +13119,12 @@
       <c r="Q26" s="4">
         <v>160</v>
       </c>
+      <c r="R26" s="4">
+        <v>199</v>
+      </c>
+      <c r="S26" s="4">
+        <v>214</v>
+      </c>
     </row>
     <row r="27" spans="1:23">
       <c r="A27" s="5" t="s">
@@ -11996,6 +13178,12 @@
       <c r="Q27" s="4">
         <v>152</v>
       </c>
+      <c r="R27" s="4">
+        <v>148</v>
+      </c>
+      <c r="S27" s="4">
+        <v>182</v>
+      </c>
     </row>
     <row r="28" spans="1:23">
       <c r="A28" s="6" t="s">
@@ -12049,6 +13237,12 @@
       <c r="Q28" s="4">
         <v>295</v>
       </c>
+      <c r="R28" s="4">
+        <v>318</v>
+      </c>
+      <c r="S28" s="4">
+        <v>345</v>
+      </c>
     </row>
     <row r="29" spans="1:23">
       <c r="A29" s="7" t="s">
@@ -12102,6 +13296,12 @@
       <c r="Q29" s="4">
         <v>552</v>
       </c>
+      <c r="R29" s="4">
+        <v>599</v>
+      </c>
+      <c r="S29" s="4">
+        <v>599</v>
+      </c>
     </row>
     <row r="30" spans="1:23">
       <c r="A30" s="8" t="s">
@@ -12155,6 +13355,12 @@
       <c r="Q30" s="4">
         <v>737</v>
       </c>
+      <c r="R30" s="4">
+        <v>755</v>
+      </c>
+      <c r="S30" s="4">
+        <v>790</v>
+      </c>
     </row>
     <row r="31" spans="1:23">
       <c r="A31" s="9" t="s">
@@ -12208,6 +13414,12 @@
       <c r="Q31" s="4">
         <v>191</v>
       </c>
+      <c r="R31" s="4">
+        <v>197</v>
+      </c>
+      <c r="S31" s="4">
+        <v>227</v>
+      </c>
     </row>
     <row r="32" spans="1:23">
       <c r="A32" s="10" t="s">
@@ -12261,6 +13473,12 @@
       <c r="Q32" s="4">
         <v>538</v>
       </c>
+      <c r="R32" s="4">
+        <v>648</v>
+      </c>
+      <c r="S32" s="4">
+        <v>684</v>
+      </c>
     </row>
     <row r="33" spans="1:23">
       <c r="A33" s="11" t="s">
@@ -12314,6 +13532,12 @@
       <c r="Q33" s="4">
         <v>787</v>
       </c>
+      <c r="R33" s="4">
+        <v>840</v>
+      </c>
+      <c r="S33" s="4">
+        <v>871</v>
+      </c>
     </row>
     <row r="34" spans="1:23">
       <c r="A34" s="12" t="s">
@@ -12367,6 +13591,12 @@
       <c r="Q34" s="4">
         <v>1367</v>
       </c>
+      <c r="R34" s="4">
+        <v>1431</v>
+      </c>
+      <c r="S34" s="4">
+        <v>1526</v>
+      </c>
     </row>
     <row r="35" spans="1:23">
       <c r="A35" s="13" t="s">
@@ -12420,6 +13650,12 @@
       <c r="Q35" s="4">
         <v>91</v>
       </c>
+      <c r="R35" s="4">
+        <v>81</v>
+      </c>
+      <c r="S35" s="4">
+        <v>110</v>
+      </c>
     </row>
     <row r="37" spans="1:23">
       <c r="A37" s="1" t="s">
@@ -12544,6 +13780,12 @@
       <c r="Q38" s="4">
         <v>97.40000000000001</v>
       </c>
+      <c r="R38" s="4">
+        <v>104.1</v>
+      </c>
+      <c r="S38" s="4">
+        <v>110.8</v>
+      </c>
     </row>
     <row r="39" spans="1:23">
       <c r="A39" s="5" t="s">
@@ -12597,6 +13839,12 @@
       <c r="Q39" s="4">
         <v>99</v>
       </c>
+      <c r="R39" s="4">
+        <v>105.7</v>
+      </c>
+      <c r="S39" s="4">
+        <v>112.9</v>
+      </c>
     </row>
     <row r="40" spans="1:23">
       <c r="A40" s="6" t="s">
@@ -12650,6 +13898,12 @@
       <c r="Q40" s="4">
         <v>167.6</v>
       </c>
+      <c r="R40" s="4">
+        <v>179.8</v>
+      </c>
+      <c r="S40" s="4">
+        <v>192.4999999999999</v>
+      </c>
     </row>
     <row r="41" spans="1:23">
       <c r="A41" s="7" t="s">
@@ -12703,6 +13957,12 @@
       <c r="Q41" s="4">
         <v>139</v>
       </c>
+      <c r="R41" s="4">
+        <v>151</v>
+      </c>
+      <c r="S41" s="4">
+        <v>163</v>
+      </c>
     </row>
     <row r="42" spans="1:23">
       <c r="A42" s="8" t="s">
@@ -12756,6 +14016,12 @@
       <c r="Q42" s="4">
         <v>364.1</v>
       </c>
+      <c r="R42" s="4">
+        <v>388.3</v>
+      </c>
+      <c r="S42" s="4">
+        <v>412.6</v>
+      </c>
     </row>
     <row r="43" spans="1:23">
       <c r="A43" s="9" t="s">
@@ -12809,6 +14075,12 @@
       <c r="Q43" s="4">
         <v>86.30000000000001</v>
       </c>
+      <c r="R43" s="4">
+        <v>93.20000000000002</v>
+      </c>
+      <c r="S43" s="4">
+        <v>100.6</v>
+      </c>
     </row>
     <row r="44" spans="1:23">
       <c r="A44" s="10" t="s">
@@ -12862,6 +14134,12 @@
       <c r="Q44" s="4">
         <v>171.3</v>
       </c>
+      <c r="R44" s="4">
+        <v>187.6</v>
+      </c>
+      <c r="S44" s="4">
+        <v>204</v>
+      </c>
     </row>
     <row r="45" spans="1:23">
       <c r="A45" s="11" t="s">
@@ -12915,6 +14193,12 @@
       <c r="Q45" s="4">
         <v>405.1</v>
       </c>
+      <c r="R45" s="4">
+        <v>430.9999999999999</v>
+      </c>
+      <c r="S45" s="4">
+        <v>456.8999999999999</v>
+      </c>
     </row>
     <row r="46" spans="1:23">
       <c r="A46" s="12" t="s">
@@ -12968,6 +14252,12 @@
       <c r="Q46" s="4">
         <v>448.4</v>
       </c>
+      <c r="R46" s="4">
+        <v>477.7</v>
+      </c>
+      <c r="S46" s="4">
+        <v>507.1</v>
+      </c>
     </row>
     <row r="47" spans="1:23">
       <c r="A47" s="13" t="s">
@@ -13021,6 +14311,12 @@
       <c r="Q47" s="4">
         <v>86.5</v>
       </c>
+      <c r="R47" s="4">
+        <v>93.3</v>
+      </c>
+      <c r="S47" s="4">
+        <v>100.6</v>
+      </c>
     </row>
     <row r="49" spans="1:23">
       <c r="A49" s="1" t="s">
@@ -13145,6 +14441,12 @@
       <c r="Q50" s="4">
         <v>10</v>
       </c>
+      <c r="R50" s="4">
+        <v>11.70588235294118</v>
+      </c>
+      <c r="S50" s="4">
+        <v>11.88888888888889</v>
+      </c>
     </row>
     <row r="51" spans="1:23">
       <c r="A51" s="5" t="s">
@@ -13198,6 +14500,12 @@
       <c r="Q51" s="4">
         <v>9.5</v>
       </c>
+      <c r="R51" s="4">
+        <v>8.705882352941176</v>
+      </c>
+      <c r="S51" s="4">
+        <v>10.11111111111111</v>
+      </c>
     </row>
     <row r="52" spans="1:23">
       <c r="A52" s="6" t="s">
@@ -13251,6 +14559,12 @@
       <c r="Q52" s="4">
         <v>18.4375</v>
       </c>
+      <c r="R52" s="4">
+        <v>18.70588235294118</v>
+      </c>
+      <c r="S52" s="4">
+        <v>19.16666666666667</v>
+      </c>
     </row>
     <row r="53" spans="1:23">
       <c r="A53" s="7" t="s">
@@ -13304,6 +14618,12 @@
       <c r="Q53" s="4">
         <v>34.5</v>
       </c>
+      <c r="R53" s="4">
+        <v>35.23529411764706</v>
+      </c>
+      <c r="S53" s="4">
+        <v>33.27777777777778</v>
+      </c>
     </row>
     <row r="54" spans="1:23">
       <c r="A54" s="8" t="s">
@@ -13357,6 +14677,12 @@
       <c r="Q54" s="4">
         <v>46.0625</v>
       </c>
+      <c r="R54" s="4">
+        <v>44.41176470588236</v>
+      </c>
+      <c r="S54" s="4">
+        <v>43.88888888888889</v>
+      </c>
     </row>
     <row r="55" spans="1:23">
       <c r="A55" s="9" t="s">
@@ -13410,6 +14736,12 @@
       <c r="Q55" s="4">
         <v>11.9375</v>
       </c>
+      <c r="R55" s="4">
+        <v>11.58823529411765</v>
+      </c>
+      <c r="S55" s="4">
+        <v>12.61111111111111</v>
+      </c>
     </row>
     <row r="56" spans="1:23">
       <c r="A56" s="10" t="s">
@@ -13463,6 +14795,12 @@
       <c r="Q56" s="4">
         <v>33.625</v>
       </c>
+      <c r="R56" s="4">
+        <v>38.11764705882353</v>
+      </c>
+      <c r="S56" s="4">
+        <v>38</v>
+      </c>
     </row>
     <row r="57" spans="1:23">
       <c r="A57" s="11" t="s">
@@ -13516,6 +14854,12 @@
       <c r="Q57" s="4">
         <v>49.1875</v>
       </c>
+      <c r="R57" s="4">
+        <v>49.41176470588236</v>
+      </c>
+      <c r="S57" s="4">
+        <v>48.38888888888889</v>
+      </c>
     </row>
     <row r="58" spans="1:23">
       <c r="A58" s="12" t="s">
@@ -13569,6 +14913,12 @@
       <c r="Q58" s="4">
         <v>85.4375</v>
       </c>
+      <c r="R58" s="4">
+        <v>84.17647058823529</v>
+      </c>
+      <c r="S58" s="4">
+        <v>84.77777777777777</v>
+      </c>
     </row>
     <row r="59" spans="1:23">
       <c r="A59" s="13" t="s">
@@ -13622,6 +14972,12 @@
       <c r="Q59" s="4">
         <v>5.6875</v>
       </c>
+      <c r="R59" s="4">
+        <v>4.764705882352941</v>
+      </c>
+      <c r="S59" s="4">
+        <v>6.111111111111111</v>
+      </c>
     </row>
     <row r="61" spans="1:23">
       <c r="A61" s="1" t="s">
@@ -13746,6 +15102,12 @@
       <c r="Q62" s="4">
         <v>6.0875</v>
       </c>
+      <c r="R62" s="4">
+        <v>6.123529411764706</v>
+      </c>
+      <c r="S62" s="4">
+        <v>6.155555555555556</v>
+      </c>
     </row>
     <row r="63" spans="1:23">
       <c r="A63" s="5" t="s">
@@ -13799,6 +15161,12 @@
       <c r="Q63" s="4">
         <v>6.1875</v>
       </c>
+      <c r="R63" s="4">
+        <v>6.21764705882353</v>
+      </c>
+      <c r="S63" s="4">
+        <v>6.272222222222222</v>
+      </c>
     </row>
     <row r="64" spans="1:23">
       <c r="A64" s="6" t="s">
@@ -13852,6 +15220,12 @@
       <c r="Q64" s="4">
         <v>10.475</v>
       </c>
+      <c r="R64" s="4">
+        <v>10.57647058823529</v>
+      </c>
+      <c r="S64" s="4">
+        <v>10.69444444444444</v>
+      </c>
     </row>
     <row r="65" spans="1:23">
       <c r="A65" s="7" t="s">
@@ -13905,6 +15279,12 @@
       <c r="Q65" s="4">
         <v>8.6875</v>
       </c>
+      <c r="R65" s="4">
+        <v>8.882352941176471</v>
+      </c>
+      <c r="S65" s="4">
+        <v>9.055555555555555</v>
+      </c>
     </row>
     <row r="66" spans="1:23">
       <c r="A66" s="8" t="s">
@@ -13958,6 +15338,12 @@
       <c r="Q66" s="4">
         <v>22.75625</v>
       </c>
+      <c r="R66" s="4">
+        <v>22.84117647058824</v>
+      </c>
+      <c r="S66" s="4">
+        <v>22.92222222222222</v>
+      </c>
     </row>
     <row r="67" spans="1:23">
       <c r="A67" s="9" t="s">
@@ -14011,6 +15397,12 @@
       <c r="Q67" s="4">
         <v>5.393750000000001</v>
       </c>
+      <c r="R67" s="4">
+        <v>5.482352941176472</v>
+      </c>
+      <c r="S67" s="4">
+        <v>5.58888888888889</v>
+      </c>
     </row>
     <row r="68" spans="1:23">
       <c r="A68" s="10" t="s">
@@ -14064,6 +15456,12 @@
       <c r="Q68" s="4">
         <v>10.70625</v>
       </c>
+      <c r="R68" s="4">
+        <v>11.03529411764706</v>
+      </c>
+      <c r="S68" s="4">
+        <v>11.33333333333334</v>
+      </c>
     </row>
     <row r="69" spans="1:23">
       <c r="A69" s="11" t="s">
@@ -14117,6 +15515,12 @@
       <c r="Q69" s="4">
         <v>25.31875</v>
       </c>
+      <c r="R69" s="4">
+        <v>25.35294117647058</v>
+      </c>
+      <c r="S69" s="4">
+        <v>25.38333333333333</v>
+      </c>
     </row>
     <row r="70" spans="1:23">
       <c r="A70" s="12" t="s">
@@ -14170,6 +15574,12 @@
       <c r="Q70" s="4">
         <v>28.025</v>
       </c>
+      <c r="R70" s="4">
+        <v>28.1</v>
+      </c>
+      <c r="S70" s="4">
+        <v>28.17222222222222</v>
+      </c>
     </row>
     <row r="71" spans="1:23">
       <c r="A71" s="13" t="s">
@@ -14223,6 +15633,12 @@
       <c r="Q71" s="4">
         <v>5.40625</v>
       </c>
+      <c r="R71" s="4">
+        <v>5.488235294117647</v>
+      </c>
+      <c r="S71" s="4">
+        <v>5.588888888888889</v>
+      </c>
     </row>
     <row r="73" spans="1:23">
       <c r="A73" s="1" t="s">
@@ -14347,6 +15763,12 @@
       <c r="Q74" s="4">
         <v>-1.587301587301587</v>
       </c>
+      <c r="R74" s="4">
+        <v>6.290322580645161</v>
+      </c>
+      <c r="S74" s="4">
+        <v>2.238805970149254</v>
+      </c>
     </row>
     <row r="75" spans="1:23">
       <c r="A75" s="5" t="s">
@@ -14400,6 +15822,12 @@
       <c r="Q75" s="4">
         <v>2.380952380952381</v>
       </c>
+      <c r="R75" s="4">
+        <v>-0.5882352941176471</v>
+      </c>
+      <c r="S75" s="4">
+        <v>5.074626865671641</v>
+      </c>
     </row>
     <row r="76" spans="1:23">
       <c r="A76" s="6" t="s">
@@ -14453,6 +15881,12 @@
       <c r="Q76" s="4">
         <v>1.785714285714286</v>
       </c>
+      <c r="R76" s="4">
+        <v>1.965811965811966</v>
+      </c>
+      <c r="S76" s="4">
+        <v>2.213114754098361</v>
+      </c>
     </row>
     <row r="77" spans="1:23">
       <c r="A77" s="7" t="s">
@@ -14506,6 +15940,12 @@
       <c r="Q77" s="4">
         <v>0.6086956521739131</v>
       </c>
+      <c r="R77" s="4">
+        <v>4.086956521739131</v>
+      </c>
+      <c r="S77" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="78" spans="1:23">
       <c r="A78" s="8" t="s">
@@ -14559,6 +15999,12 @@
       <c r="Q78" s="4">
         <v>2.73109243697479</v>
       </c>
+      <c r="R78" s="4">
+        <v>0.7468879668049793</v>
+      </c>
+      <c r="S78" s="4">
+        <v>1.446280991735537</v>
+      </c>
     </row>
     <row r="79" spans="1:23">
       <c r="A79" s="9" t="s">
@@ -14612,6 +16058,12 @@
       <c r="Q79" s="4">
         <v>2.34375</v>
       </c>
+      <c r="R79" s="4">
+        <v>0.8695652173913043</v>
+      </c>
+      <c r="S79" s="4">
+        <v>4.347826086956522</v>
+      </c>
     </row>
     <row r="80" spans="1:23">
       <c r="A80" s="10" t="s">
@@ -14665,6 +16117,12 @@
       <c r="Q80" s="4">
         <v>4.615384615384615</v>
       </c>
+      <c r="R80" s="4">
+        <v>7.18954248366013</v>
+      </c>
+      <c r="S80" s="4">
+        <v>2.208588957055214</v>
+      </c>
     </row>
     <row r="81" spans="1:23">
       <c r="A81" s="11" t="s">
@@ -14718,6 +16176,12 @@
       <c r="Q81" s="4">
         <v>1.712062256809339</v>
       </c>
+      <c r="R81" s="4">
+        <v>2.054263565891473</v>
+      </c>
+      <c r="S81" s="4">
+        <v>1.196911196911197</v>
+      </c>
     </row>
     <row r="82" spans="1:23">
       <c r="A82" s="12" t="s">
@@ -14771,6 +16235,12 @@
       <c r="Q82" s="4">
         <v>1.580756013745704</v>
       </c>
+      <c r="R82" s="4">
+        <v>2.191780821917808</v>
+      </c>
+      <c r="S82" s="4">
+        <v>3.242320819112628</v>
+      </c>
     </row>
     <row r="83" spans="1:23">
       <c r="A83" s="13" t="s">
@@ -14824,6 +16294,12 @@
       <c r="Q83" s="4">
         <v>-5</v>
       </c>
+      <c r="R83" s="4">
+        <v>-1.449275362318841</v>
+      </c>
+      <c r="S83" s="4">
+        <v>4.264705882352941</v>
+      </c>
     </row>
     <row r="85" spans="1:23">
       <c r="A85" s="1" t="s">
@@ -14948,6 +16424,12 @@
       <c r="Q86" s="4">
         <v>1.74863387978142</v>
       </c>
+      <c r="R86" s="4">
+        <v>2.036847492323439</v>
+      </c>
+      <c r="S86" s="4">
+        <v>2.049808429118773</v>
+      </c>
     </row>
     <row r="87" spans="1:23">
       <c r="A87" s="5" t="s">
@@ -15001,6 +16483,12 @@
       <c r="Q87" s="4">
         <v>1.543147208121827</v>
       </c>
+      <c r="R87" s="4">
+        <v>1.405508072174739</v>
+      </c>
+      <c r="S87" s="4">
+        <v>1.625</v>
+      </c>
     </row>
     <row r="88" spans="1:23">
       <c r="A88" s="6" t="s">
@@ -15054,6 +16542,12 @@
       <c r="Q88" s="4">
         <v>1.778179626280892</v>
       </c>
+      <c r="R88" s="4">
+        <v>1.790540540540541</v>
+      </c>
+      <c r="S88" s="4">
+        <v>1.817702845100106</v>
+      </c>
     </row>
     <row r="89" spans="1:23">
       <c r="A89" s="7" t="s">
@@ -15107,6 +16601,12 @@
       <c r="Q89" s="4">
         <v>4.110201042442293</v>
       </c>
+      <c r="R89" s="4">
+        <v>4.108367626886145</v>
+      </c>
+      <c r="S89" s="4">
+        <v>4.108367626886145</v>
+      </c>
     </row>
     <row r="90" spans="1:23">
       <c r="A90" s="8" t="s">
@@ -15160,6 +16660,12 @@
       <c r="Q90" s="4">
         <v>2.035349351008009</v>
       </c>
+      <c r="R90" s="4">
+        <v>1.954945624029</v>
+      </c>
+      <c r="S90" s="4">
+        <v>1.92495126705653</v>
+      </c>
     </row>
     <row r="91" spans="1:23">
       <c r="A91" s="9" t="s">
@@ -15213,6 +16719,12 @@
       <c r="Q91" s="4">
         <v>2.423857868020304</v>
       </c>
+      <c r="R91" s="4">
+        <v>2.298716452742123</v>
+      </c>
+      <c r="S91" s="4">
+        <v>2.451403887688984</v>
+      </c>
     </row>
     <row r="92" spans="1:23">
       <c r="A92" s="10" t="s">
@@ -15266,6 +16778,12 @@
       <c r="Q92" s="4">
         <v>3.260606060606061</v>
       </c>
+      <c r="R92" s="4">
+        <v>3.594009983361065</v>
+      </c>
+      <c r="S92" s="4">
+        <v>3.479145473041709</v>
+      </c>
     </row>
     <row r="93" spans="1:23">
       <c r="A93" s="11" t="s">
@@ -15319,6 +16837,12 @@
       <c r="Q93" s="4">
         <v>1.946092977250248</v>
       </c>
+      <c r="R93" s="4">
+        <v>1.95258019525802</v>
+      </c>
+      <c r="S93" s="4">
+        <v>1.9096689322517</v>
+      </c>
     </row>
     <row r="94" spans="1:23">
       <c r="A94" s="12" t="s">
@@ -15372,6 +16896,12 @@
       <c r="Q94" s="4">
         <v>3.061590145576708</v>
       </c>
+      <c r="R94" s="4">
+        <v>3.00819844439773</v>
+      </c>
+      <c r="S94" s="4">
+        <v>3.021782178217822</v>
+      </c>
     </row>
     <row r="95" spans="1:23">
       <c r="A95" s="13" t="s">
@@ -15424,6 +16954,12 @@
       </c>
       <c r="Q95" s="4">
         <v>1.074380165289256</v>
+      </c>
+      <c r="R95" s="4">
+        <v>0.8842794759825326</v>
+      </c>
+      <c r="S95" s="4">
+        <v>1.117886178861789</v>
       </c>
     </row>
   </sheetData>

</xml_diff>